<commit_message>
Refer to Excel Sheet
</commit_message>
<xml_diff>
--- a/Rest Services.xlsx
+++ b/Rest Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\IBM FullStack Training\Final Project\JavaFullStackProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FACCD3A-41EF-41D0-93D8-BE2CF4D9AF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A9D02-7A29-4B8F-B93D-800BC2954EE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2712" yWindow="2208" windowWidth="19716" windowHeight="10152" tabRatio="290" xr2:uid="{4AA07E8F-24ED-4EA0-B36A-7BFACD69731D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="290" xr2:uid="{4AA07E8F-24ED-4EA0-B36A-7BFACD69731D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
 </t>
   </si>
   <si>
-    <t>/app/admin/login</t>
-  </si>
-  <si>
     <t>EX-001</t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>Know Your Booking Status</t>
+  </si>
+  <si>
+    <t>/app/user/login</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D0ABD9-72D5-49BE-82B2-5310752EDAC5}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,10 +927,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>7</v>
@@ -954,13 +954,13 @@
         <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
@@ -982,14 +982,14 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="4" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>39</v>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1047,7 +1047,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>12</v>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1083,7 +1083,7 @@
         <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
@@ -1099,7 +1099,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -1112,7 +1112,7 @@
         <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="234" x14ac:dyDescent="0.3">
@@ -1132,7 +1132,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>12</v>
@@ -1147,7 +1147,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="144" x14ac:dyDescent="0.3">
@@ -1167,7 +1167,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
@@ -1190,13 +1190,13 @@
         <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="144" x14ac:dyDescent="0.3">
@@ -1210,7 +1210,7 @@
         <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>55</v>
@@ -1222,7 +1222,7 @@
         <v>56</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="144" x14ac:dyDescent="0.3">
@@ -1242,7 +1242,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
@@ -1257,102 +1257,102 @@
         <v>56</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>12</v>
@@ -1360,58 +1360,58 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
@@ -1424,7 +1424,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>12</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="20" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>13</v>
@@ -1449,13 +1449,13 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>15</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="21" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>13</v>
@@ -1474,13 +1474,13 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="22" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>9</v>
@@ -1517,17 +1517,17 @@
     </row>
     <row r="23" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1541,18 +1541,18 @@
     </row>
     <row r="24" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>

</xml_diff>